<commit_message>
TOOOO much to say what i have changed, so you have to look at it :)
</commit_message>
<xml_diff>
--- a/assets/insta_search_found.xlsx
+++ b/assets/insta_search_found.xlsx
@@ -1,63 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Phthon\Projects\Instagram_like_follow\assets\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="11400" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="16980" yWindow="105" windowWidth="14805" windowHeight="8010" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames>
     <definedName name="A2000000">Sheet1!$A$1000000</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>Master ID</t>
-  </si>
-  <si>
-    <t>Status</t>
-  </si>
-  <si>
-    <t>bcbilliofficial</t>
-  </si>
-  <si>
-    <t>tapishmiddha</t>
-  </si>
-  <si>
-    <t>visionacademy01</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -88,23 +60,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -394,43 +357,117 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B8" sqref="B5:B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="30.7109375" customWidth="1"/>
-    <col min="2" max="2" width="18.5703125" customWidth="1"/>
+    <col width="30.7109375" customWidth="1" min="1" max="1"/>
+    <col width="18.5703125" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>Master ID</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Status</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>pearl.what.is.this.behaviour</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>bcbilliofficial</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>aman.gupta.09</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>dhattarwalaman</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Benc4n</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>tumblrindeed</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>thesavagebean</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>OK</t>
+        </is>
       </c>
     </row>
   </sheetData>

</xml_diff>